<commit_message>
Finished adding the department names to the eval template at upload
can now see all the departments an eval template belongs to at upload
and after when clicking the view.

Fixed the view showing the departments more than once.
</commit_message>
<xml_diff>
--- a/WebBasedEvaluations/Documents/Upload_Evaluation_-_EVAL-001.xlsx
+++ b/WebBasedEvaluations/Documents/Upload_Evaluation_-_EVAL-001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\Fall-2022-Group-3-Web-Evaluation\WebBasedEvaluations\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E0C37C-0C35-41AC-9B30-46FFFF9B7225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DE149A-7388-4463-AA30-2370611A48A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3FAD3DD6-7A1D-42CB-BC54-8CFE443C5D15}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3FAD3DD6-7A1D-42CB-BC54-8CFE443C5D15}"/>
   </bookViews>
   <sheets>
     <sheet name="Eval_format" sheetId="1" r:id="rId1"/>
@@ -4873,7 +4873,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A9"/>
+      <selection activeCell="A10" sqref="A10:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>